<commit_message>
Added the creation of the user and the generation of the token
</commit_message>
<xml_diff>
--- a/AssessmentOI/assessment/static/Template v01.2.xlsx
+++ b/AssessmentOI/assessment/static/Template v01.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefano/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefano/Dropbox/NewDev/AssessmentOI/AssessmentOI/assessment/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F637BEFD-AB86-1E43-AF38-8ADE19F76F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E2F5E4-999E-E443-B2A1-DF24A19927CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{BEC74A21-4066-9F46-9A91-B583390417DD}"/>
   </bookViews>
@@ -648,7 +648,7 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -715,7 +715,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -724,61 +724,61 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
       </c>
       <c r="O2" t="str">
         <f>CONCATENATE("[",P2,Q2,R2,S2,T2,"]")</f>
         <v>[answer_1,answer_2,answer_3,]</v>
       </c>
       <c r="P2" t="str">
-        <f>IF(J2="Yes",CONCATENATE(J$1,","),"")</f>
+        <f>IF(E2="Yes",CONCATENATE(J$1,","),"")</f>
         <v>answer_1,</v>
       </c>
       <c r="Q2" t="str">
-        <f>IF(K2="Yes",CONCATENATE(K$1,","),"")</f>
+        <f>IF(F2="Yes",CONCATENATE(K$1,","),"")</f>
         <v>answer_2,</v>
       </c>
       <c r="R2" t="str">
-        <f>IF(L2="Yes",CONCATENATE(L$1,","),"")</f>
+        <f>IF(G2="Yes",CONCATENATE(L$1,","),"")</f>
         <v>answer_3,</v>
       </c>
       <c r="S2" t="str">
-        <f>IF(M2="Yes",CONCATENATE(M$1,","),"")</f>
+        <f>IF(H2="Yes",CONCATENATE(M$1,","),"")</f>
         <v/>
       </c>
       <c r="T2" t="str">
-        <f>IF(N2="Yes",CONCATENATE(N$1,","),"")</f>
+        <f>IF(I2="Yes",CONCATENATE(N$1,","),"")</f>
         <v/>
       </c>
       <c r="U2" t="str">
-        <f>IF(I2="Yes",I$1,"")</f>
+        <f>IF(N2="Yes",I$1,"")</f>
         <v/>
       </c>
       <c r="V2" t="s">
@@ -799,61 +799,61 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
+      <c r="L3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
+      <c r="N3" t="s">
         <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" t="s">
-        <v>15</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" ref="O3:O10" si="0">CONCATENATE("[",P3,Q3,R3,S3,T3,"]")</f>
         <v>[answer_1,answer_2,answer_4,]</v>
       </c>
       <c r="P3" t="str">
-        <f>IF(J3="Yes",CONCATENATE(J$1,","),"")</f>
+        <f>IF(E3="Yes",CONCATENATE(J$1,","),"")</f>
         <v>answer_1,</v>
       </c>
       <c r="Q3" t="str">
-        <f>IF(K3="Yes",CONCATENATE(K$1,","),"")</f>
+        <f>IF(F3="Yes",CONCATENATE(K$1,","),"")</f>
         <v>answer_2,</v>
       </c>
       <c r="R3" t="str">
-        <f>IF(L3="Yes",CONCATENATE(L$1,","),"")</f>
+        <f>IF(G3="Yes",CONCATENATE(L$1,","),"")</f>
         <v/>
       </c>
       <c r="S3" t="str">
-        <f>IF(M3="Yes",CONCATENATE(M$1,","),"")</f>
+        <f>IF(H3="Yes",CONCATENATE(M$1,","),"")</f>
         <v>answer_4,</v>
       </c>
       <c r="T3" t="str">
-        <f>IF(N3="Yes",CONCATENATE(N$1,","),"")</f>
+        <f>IF(I3="Yes",CONCATENATE(N$1,","),"")</f>
         <v/>
       </c>
       <c r="U3" t="str">
-        <f>IF(I3="Yes",I$1,"")</f>
+        <f>IF(N3="Yes",I$1,"")</f>
         <v/>
       </c>
       <c r="V3" t="s">
@@ -874,61 +874,61 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
+      <c r="M4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" t="s">
+      <c r="N4" t="s">
         <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" t="s">
-        <v>15</v>
       </c>
       <c r="O4" t="str">
         <f t="shared" si="0"/>
         <v>[answer_1,answer_3,answer_4,]</v>
       </c>
       <c r="P4" t="str">
-        <f>IF(J4="Yes",CONCATENATE(J$1,","),"")</f>
+        <f>IF(E4="Yes",CONCATENATE(J$1,","),"")</f>
         <v>answer_1,</v>
       </c>
       <c r="Q4" t="str">
-        <f>IF(K4="Yes",CONCATENATE(K$1,","),"")</f>
+        <f>IF(F4="Yes",CONCATENATE(K$1,","),"")</f>
         <v/>
       </c>
       <c r="R4" t="str">
-        <f>IF(L4="Yes",CONCATENATE(L$1,","),"")</f>
+        <f>IF(G4="Yes",CONCATENATE(L$1,","),"")</f>
         <v>answer_3,</v>
       </c>
       <c r="S4" t="str">
-        <f>IF(M4="Yes",CONCATENATE(M$1,","),"")</f>
+        <f>IF(H4="Yes",CONCATENATE(M$1,","),"")</f>
         <v>answer_4,</v>
       </c>
       <c r="T4" t="str">
-        <f>IF(N4="Yes",CONCATENATE(N$1,","),"")</f>
+        <f>IF(I4="Yes",CONCATENATE(N$1,","),"")</f>
         <v/>
       </c>
       <c r="U4" t="str">
-        <f>IF(I4="Yes",I$1,"")</f>
+        <f>IF(N4="Yes",I$1,"")</f>
         <v/>
       </c>
       <c r="V4" t="s">
@@ -949,65 +949,65 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="K5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="L5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" t="s">
+      <c r="M5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" t="s">
+      <c r="N5" t="s">
         <v>23</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" t="s">
-        <v>15</v>
       </c>
       <c r="O5" t="str">
         <f t="shared" si="0"/>
         <v>[answer_1,answer_2,answer_3,]</v>
       </c>
       <c r="P5" t="str">
-        <f>IF(J5="Yes",CONCATENATE(J$1,","),"")</f>
+        <f>IF(E5="Yes",CONCATENATE(J$1,","),"")</f>
         <v>answer_1,</v>
       </c>
       <c r="Q5" t="str">
-        <f>IF(K5="Yes",CONCATENATE(K$1,","),"")</f>
+        <f>IF(F5="Yes",CONCATENATE(K$1,","),"")</f>
         <v>answer_2,</v>
       </c>
       <c r="R5" t="str">
-        <f>IF(L5="Yes",CONCATENATE(L$1,","),"")</f>
+        <f>IF(G5="Yes",CONCATENATE(L$1,","),"")</f>
         <v>answer_3,</v>
       </c>
       <c r="S5" t="str">
-        <f>IF(M5="Yes",CONCATENATE(M$1,","),"")</f>
+        <f>IF(H5="Yes",CONCATENATE(M$1,","),"")</f>
         <v/>
       </c>
       <c r="T5" t="str">
-        <f>IF(N5="Yes",CONCATENATE(N$1,","),"")</f>
+        <f>IF(I5="Yes",CONCATENATE(N$1,","),"")</f>
         <v/>
       </c>
       <c r="U5" t="str">
-        <f>IF(I5="Yes",I$1,"")</f>
+        <f>IF(N5="Yes",I$1,"")</f>
         <v/>
       </c>
       <c r="V5" t="str">
-        <f t="shared" ref="V2:V10" si="1">IF(O5="Yes",O$1,"")</f>
+        <f t="shared" ref="V5:V10" si="1">IF(O5="Yes",O$1,"")</f>
         <v/>
       </c>
     </row>
@@ -1025,61 +1025,61 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+      <c r="K6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" t="s">
+      <c r="L6" t="s">
         <v>21</v>
       </c>
-      <c r="H6" t="s">
+      <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="I6" t="s">
+      <c r="N6" t="s">
         <v>23</v>
-      </c>
-      <c r="J6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" t="s">
-        <v>14</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="0"/>
         <v>[answer_1,answer_3,answer_5,]</v>
       </c>
       <c r="P6" t="str">
-        <f>IF(J6="Yes",CONCATENATE(J$1,","),"")</f>
+        <f>IF(E6="Yes",CONCATENATE(J$1,","),"")</f>
         <v>answer_1,</v>
       </c>
       <c r="Q6" t="str">
-        <f>IF(K6="Yes",CONCATENATE(K$1,","),"")</f>
+        <f>IF(F6="Yes",CONCATENATE(K$1,","),"")</f>
         <v/>
       </c>
       <c r="R6" t="str">
-        <f>IF(L6="Yes",CONCATENATE(L$1,","),"")</f>
+        <f>IF(G6="Yes",CONCATENATE(L$1,","),"")</f>
         <v>answer_3,</v>
       </c>
       <c r="S6" t="str">
-        <f>IF(M6="Yes",CONCATENATE(M$1,","),"")</f>
+        <f>IF(H6="Yes",CONCATENATE(M$1,","),"")</f>
         <v/>
       </c>
       <c r="T6" t="str">
-        <f>IF(N6="Yes",CONCATENATE(N$1,","),"")</f>
+        <f>IF(I6="Yes",CONCATENATE(N$1,","),"")</f>
         <v>answer_5,</v>
       </c>
       <c r="U6" t="str">
-        <f>IF(I6="Yes",I$1,"")</f>
+        <f>IF(N6="Yes",I$1,"")</f>
         <v/>
       </c>
       <c r="V6" t="str">
@@ -1101,61 +1101,61 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
+      <c r="K7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
+      <c r="L7" t="s">
         <v>21</v>
       </c>
-      <c r="H7" t="s">
+      <c r="M7" t="s">
         <v>22</v>
       </c>
-      <c r="I7" t="s">
+      <c r="N7" t="s">
         <v>23</v>
-      </c>
-      <c r="J7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" t="s">
-        <v>15</v>
-      </c>
-      <c r="N7" t="s">
-        <v>15</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="0"/>
         <v>[answer_1,answer_2,answer_3,]</v>
       </c>
       <c r="P7" t="str">
-        <f>IF(J7="Yes",CONCATENATE(J$1,","),"")</f>
+        <f>IF(E7="Yes",CONCATENATE(J$1,","),"")</f>
         <v>answer_1,</v>
       </c>
       <c r="Q7" t="str">
-        <f>IF(K7="Yes",CONCATENATE(K$1,","),"")</f>
+        <f>IF(F7="Yes",CONCATENATE(K$1,","),"")</f>
         <v>answer_2,</v>
       </c>
       <c r="R7" t="str">
-        <f>IF(L7="Yes",CONCATENATE(L$1,","),"")</f>
+        <f>IF(G7="Yes",CONCATENATE(L$1,","),"")</f>
         <v>answer_3,</v>
       </c>
       <c r="S7" t="str">
-        <f>IF(M7="Yes",CONCATENATE(M$1,","),"")</f>
+        <f>IF(H7="Yes",CONCATENATE(M$1,","),"")</f>
         <v/>
       </c>
       <c r="T7" t="str">
-        <f>IF(N7="Yes",CONCATENATE(N$1,","),"")</f>
+        <f>IF(I7="Yes",CONCATENATE(N$1,","),"")</f>
         <v/>
       </c>
       <c r="U7" t="str">
-        <f>IF(I7="Yes",I$1,"")</f>
+        <f>IF(N7="Yes",I$1,"")</f>
         <v/>
       </c>
       <c r="V7" t="str">
@@ -1177,61 +1177,61 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
+      <c r="K8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
+      <c r="L8" t="s">
         <v>21</v>
       </c>
-      <c r="H8" t="s">
+      <c r="M8" t="s">
         <v>22</v>
       </c>
-      <c r="I8" t="s">
+      <c r="N8" t="s">
         <v>23</v>
-      </c>
-      <c r="J8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" t="s">
-        <v>15</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="0"/>
         <v>[answer_1,answer_2,answer_3,]</v>
       </c>
       <c r="P8" t="str">
-        <f>IF(J8="Yes",CONCATENATE(J$1,","),"")</f>
+        <f>IF(E8="Yes",CONCATENATE(J$1,","),"")</f>
         <v>answer_1,</v>
       </c>
       <c r="Q8" t="str">
-        <f>IF(K8="Yes",CONCATENATE(K$1,","),"")</f>
+        <f>IF(F8="Yes",CONCATENATE(K$1,","),"")</f>
         <v>answer_2,</v>
       </c>
       <c r="R8" t="str">
-        <f>IF(L8="Yes",CONCATENATE(L$1,","),"")</f>
+        <f>IF(G8="Yes",CONCATENATE(L$1,","),"")</f>
         <v>answer_3,</v>
       </c>
       <c r="S8" t="str">
-        <f>IF(M8="Yes",CONCATENATE(M$1,","),"")</f>
+        <f>IF(H8="Yes",CONCATENATE(M$1,","),"")</f>
         <v/>
       </c>
       <c r="T8" t="str">
-        <f>IF(N8="Yes",CONCATENATE(N$1,","),"")</f>
+        <f>IF(I8="Yes",CONCATENATE(N$1,","),"")</f>
         <v/>
       </c>
       <c r="U8" t="str">
-        <f>IF(I8="Yes",I$1,"")</f>
+        <f>IF(N8="Yes",I$1,"")</f>
         <v/>
       </c>
       <c r="V8" t="str">
@@ -1253,61 +1253,61 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
         <v>19</v>
       </c>
-      <c r="F9" t="s">
+      <c r="K9" t="s">
         <v>20</v>
       </c>
-      <c r="G9" t="s">
+      <c r="L9" t="s">
         <v>21</v>
       </c>
-      <c r="H9" t="s">
+      <c r="M9" t="s">
         <v>22</v>
       </c>
-      <c r="I9" t="s">
+      <c r="N9" t="s">
         <v>23</v>
-      </c>
-      <c r="J9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N9" t="s">
-        <v>15</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="0"/>
         <v>[answer_1,answer_2,answer_3,]</v>
       </c>
       <c r="P9" t="str">
-        <f>IF(J9="Yes",CONCATENATE(J$1,","),"")</f>
+        <f>IF(E9="Yes",CONCATENATE(J$1,","),"")</f>
         <v>answer_1,</v>
       </c>
       <c r="Q9" t="str">
-        <f>IF(K9="Yes",CONCATENATE(K$1,","),"")</f>
+        <f>IF(F9="Yes",CONCATENATE(K$1,","),"")</f>
         <v>answer_2,</v>
       </c>
       <c r="R9" t="str">
-        <f>IF(L9="Yes",CONCATENATE(L$1,","),"")</f>
+        <f>IF(G9="Yes",CONCATENATE(L$1,","),"")</f>
         <v>answer_3,</v>
       </c>
       <c r="S9" t="str">
-        <f>IF(M9="Yes",CONCATENATE(M$1,","),"")</f>
+        <f>IF(H9="Yes",CONCATENATE(M$1,","),"")</f>
         <v/>
       </c>
       <c r="T9" t="str">
-        <f>IF(N9="Yes",CONCATENATE(N$1,","),"")</f>
+        <f>IF(I9="Yes",CONCATENATE(N$1,","),"")</f>
         <v/>
       </c>
       <c r="U9" t="str">
-        <f>IF(I9="Yes",I$1,"")</f>
+        <f>IF(N9="Yes",I$1,"")</f>
         <v/>
       </c>
       <c r="V9" t="str">
@@ -1329,61 +1329,61 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
         <v>19</v>
       </c>
-      <c r="F10" t="s">
+      <c r="K10" t="s">
         <v>20</v>
       </c>
-      <c r="G10" t="s">
+      <c r="L10" t="s">
         <v>21</v>
       </c>
-      <c r="H10" t="s">
+      <c r="M10" t="s">
         <v>22</v>
       </c>
-      <c r="I10" t="s">
+      <c r="N10" t="s">
         <v>23</v>
-      </c>
-      <c r="J10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M10" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" t="s">
-        <v>15</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="0"/>
         <v>[answer_1,answer_2,answer_3,]</v>
       </c>
       <c r="P10" t="str">
-        <f>IF(J10="Yes",CONCATENATE(J$1,","),"")</f>
+        <f>IF(E10="Yes",CONCATENATE(J$1,","),"")</f>
         <v>answer_1,</v>
       </c>
       <c r="Q10" t="str">
-        <f>IF(K10="Yes",CONCATENATE(K$1,","),"")</f>
+        <f>IF(F10="Yes",CONCATENATE(K$1,","),"")</f>
         <v>answer_2,</v>
       </c>
       <c r="R10" t="str">
-        <f>IF(L10="Yes",CONCATENATE(L$1,","),"")</f>
+        <f>IF(G10="Yes",CONCATENATE(L$1,","),"")</f>
         <v>answer_3,</v>
       </c>
       <c r="S10" t="str">
-        <f>IF(M10="Yes",CONCATENATE(M$1,","),"")</f>
+        <f>IF(H10="Yes",CONCATENATE(M$1,","),"")</f>
         <v/>
       </c>
       <c r="T10" t="str">
-        <f>IF(N10="Yes",CONCATENATE(N$1,","),"")</f>
+        <f>IF(I10="Yes",CONCATENATE(N$1,","),"")</f>
         <v/>
       </c>
       <c r="U10" t="str">
-        <f>IF(I10="Yes",I$1,"")</f>
+        <f>IF(N10="Yes",I$1,"")</f>
         <v/>
       </c>
       <c r="V10" t="str">
@@ -1399,7 +1399,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10" xr:uid="{C59676B5-AAAA-6A42-A1D9-38BC63182E32}">
       <formula1>"2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:N10" xr:uid="{C0219B36-7269-004E-91EE-FFE5709D8E59}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:I10" xr:uid="{C0219B36-7269-004E-91EE-FFE5709D8E59}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10" xr:uid="{258C423B-FD63-D145-AA5E-2C5D68F85DB0}">

</xml_diff>